<commit_message>
some more Amazon OA questions
</commit_message>
<xml_diff>
--- a/Leetcode record for Shiyun.xlsx
+++ b/Leetcode record for Shiyun.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11210" windowHeight="5660" tabRatio="779" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11210" windowHeight="5660" tabRatio="779"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Record 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3288" uniqueCount="800">
   <si>
     <t>Two Pointers</t>
   </si>
@@ -5183,12 +5183,57 @@
 poll() // remove the head
 remove(Object o)
 You can't traverse a priority queue in that order because of the underlying implementation (I think it's min-heap in Java). 
+Initial capacity is just initial, PQ's capacity can grow later, use TreeSet if you want to pollFirst() pollLast()
 for (Event e : pq)
 doesn't iterate in the priority order.
 while(!pq.isEmpty()){
   Event e = pq.poll();
 }
 This works but empties the queue.</t>
+  </si>
+  <si>
+    <t>TreeSet</t>
+  </si>
+  <si>
+    <t>TreeSet(Comparator&lt;? super E&gt; comparator)
+pollFirst()
+Retrieves and removes the first (lowest) element, or returns null if this set is empty.
+pollLast()
+Retrieves and removes the last (highest) element, or returns null if this set is empty.
+//iterate
+TreeSet&lt;E&gt; ts;
+for(E e : ts) {}</t>
+  </si>
+  <si>
+    <t>Course Schedule II</t>
+  </si>
+  <si>
+    <t>There are a total of n courses you have to take, labeled from 0 to n - 1.
+Some courses may have prerequisites, for example to take course 0 you have to first take course 1, which is expressed as a pair: [0,1]
+Given the total number of courses and a list of prerequisite pairs, return the ordering of courses you should take to finish all courses.
+There may be multiple correct orders, you just need to return one of them. If it is impossible to finish all courses, return an empty array.
+For example:
+2, [[1,0]]
+There are a total of 2 courses to take. To take course 1 you should have finished course 0. So the correct course order is [0,1]
+4, [[1,0],[2,0],[3,1],[3,2]]
+There are a total of 4 courses to take. To take course 3 you should have finished both courses 1 and 2. Both courses 1 and 2 should be taken after you finished course 0. So one correct course order is [0,1,2,3]. Another correct ordering is[0,2,1,3].</t>
+  </si>
+  <si>
+    <t>Topological Sort</t>
+  </si>
+  <si>
+    <t>If input has duplicate edges, need to handle this.
+test case: 10, [[5,8],[3,5],[1,9],[4,5],[0,2],[1,9],[7,8],[4,9]]
+This problem is equivalent to finding the topological order in a directed graph. If a cycle exists, no topological ordering exists and therefore it will be impossible to take all courses.</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>dfs, drown visited islands!</t>
+  </si>
+  <si>
+    <t>Union Find</t>
   </si>
 </sst>
 </file>
@@ -21356,12 +21401,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ239"/>
+  <dimension ref="A1:AL239"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="A232" sqref="A232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21382,7 +21427,7 @@
     <col min="34" max="35" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -21491,8 +21536,14 @@
       <c r="AJ1" s="24" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK1" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -21539,7 +21590,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:36" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -21594,7 +21645,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -21639,7 +21690,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -21684,7 +21735,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
     </row>
-    <row r="6" spans="1:36" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -21729,7 +21780,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:36" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -21778,7 +21829,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
     </row>
-    <row r="8" spans="1:36" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -21825,7 +21876,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
     </row>
-    <row r="9" spans="1:36" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -21879,7 +21930,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:36" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -21929,7 +21980,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:36" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -21985,7 +22036,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
     </row>
-    <row r="12" spans="1:36" ht="174" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" ht="174" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -22041,7 +22092,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
     </row>
-    <row r="13" spans="1:36" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -22097,7 +22148,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:36" ht="242.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" ht="242.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -22147,7 +22198,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
     </row>
-    <row r="15" spans="1:36" ht="116" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" ht="116" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -22195,7 +22246,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:36" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -28640,6 +28691,15 @@
       <c r="G215" s="9">
         <v>42752</v>
       </c>
+      <c r="H215" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I215" s="9">
+        <v>42801</v>
+      </c>
+      <c r="J215" s="8" t="s">
+        <v>318</v>
+      </c>
       <c r="P215" s="8" t="s">
         <v>5</v>
       </c>
@@ -28938,7 +28998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:31" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:38" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A225" s="8" t="s">
         <v>30</v>
       </c>
@@ -28970,7 +29030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:31" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:38" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A226" s="8" t="s">
         <v>30</v>
       </c>
@@ -28997,7 +29057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:31" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A227" s="8" t="s">
         <v>95</v>
       </c>
@@ -29020,7 +29080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:31" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:38" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A228" s="8" t="s">
         <v>46</v>
       </c>
@@ -29040,7 +29100,7 @@
         <v>42780</v>
       </c>
     </row>
-    <row r="229" spans="1:31" ht="87" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:38" ht="87" x14ac:dyDescent="0.35">
       <c r="A229" s="8" t="s">
         <v>46</v>
       </c>
@@ -29063,7 +29123,76 @@
         <v>42791</v>
       </c>
     </row>
-    <row r="239" spans="1:31" ht="174" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:38" ht="290" x14ac:dyDescent="0.35">
+      <c r="A230" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B230" s="8">
+        <v>210</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="D230" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="E230" s="13" t="s">
+        <v>796</v>
+      </c>
+      <c r="F230" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G230" s="9">
+        <v>42802</v>
+      </c>
+      <c r="J230" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB230" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK230" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:38" ht="29" x14ac:dyDescent="0.35">
+      <c r="A231" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B231" s="8">
+        <v>200</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="E231" s="12" t="s">
+        <v>798</v>
+      </c>
+      <c r="F231" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G231" s="9">
+        <v>42803</v>
+      </c>
+      <c r="J231" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB231" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A232" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B232" s="8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="239" spans="1:38" ht="174" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>30</v>
       </c>
@@ -41061,10 +41190,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41125,7 +41254,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>257</v>
       </c>
@@ -41177,6 +41306,14 @@
       </c>
       <c r="C11" s="8" t="s">
         <v>741</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>